<commit_message>
fix BOM to add missing crystal (!)
</commit_message>
<xml_diff>
--- a/hardware/tottag/rev_f/tottag_bom.xlsx
+++ b/hardware/tottag/rev_f/tottag_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/code/lab11/totternary/hardware/tottag/rev_f/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E2DEE282-4DA9-A443-B9CE-16BB19F91BAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D57CB6C-B24E-E441-9E9B-ADB8E735D85A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="14160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="18760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tottag_bom" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="385">
   <si>
     <t>Qty</t>
   </si>
@@ -1165,6 +1165,21 @@
   </si>
   <si>
     <t>IC RTC CLK/CALENDAR SPI 16-QFN</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>ABS07</t>
+  </si>
+  <si>
+    <t>ABS07-32.768KHZ-7-T</t>
+  </si>
+  <si>
+    <t>CRYSTAL 32.7680KHZ 7PF SMD</t>
+  </si>
+  <si>
+    <t>535-9543-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1966,10 +1981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4078,122 +4093,159 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A57">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>323</v>
+        <v>380</v>
       </c>
       <c r="C57" t="s">
-        <v>324</v>
-      </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="5" t="s">
-        <v>325</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="5"/>
       <c r="F57" t="s">
-        <v>324</v>
+        <v>382</v>
       </c>
       <c r="G57" t="s">
-        <v>326</v>
+        <v>381</v>
       </c>
       <c r="H57" t="s">
-        <v>327</v>
+        <v>298</v>
+      </c>
+      <c r="I57" t="s">
+        <v>383</v>
+      </c>
+      <c r="J57" t="s">
+        <v>384</v>
+      </c>
+      <c r="K57" t="s">
+        <v>154</v>
+      </c>
+      <c r="L57" t="s">
+        <v>382</v>
       </c>
       <c r="N57"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A58">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C58" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="5" t="s">
         <v>325</v>
       </c>
       <c r="F58" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="G58" t="s">
-        <v>330</v>
+        <v>326</v>
+      </c>
+      <c r="H58" t="s">
+        <v>327</v>
       </c>
       <c r="N58"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A59">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C59" t="s">
-        <v>332</v>
-      </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="5" t="s">
         <v>325</v>
       </c>
       <c r="F59" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G59" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="N59"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C60" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4" t="s">
         <v>325</v>
       </c>
       <c r="F60" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G60" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N60"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C61" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
         <v>325</v>
       </c>
       <c r="F61" t="s">
+        <v>335</v>
+      </c>
+      <c r="G61" t="s">
+        <v>336</v>
+      </c>
+      <c r="N61"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>337</v>
+      </c>
+      <c r="C62" t="s">
         <v>338</v>
       </c>
-      <c r="G61" t="s">
+      <c r="D62" s="5"/>
+      <c r="E62" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F62" t="s">
+        <v>338</v>
+      </c>
+      <c r="G62" t="s">
         <v>339</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H62" t="s">
         <v>340</v>
       </c>
-      <c r="N61"/>
+      <c r="N62"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D53:D58 D2:D10 D34:D50 D12:D29">
+  <conditionalFormatting sqref="D2:D10 D34:D50 D12:D29 D53:D59">
     <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -4201,12 +4253,12 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53:E58 E2:E10 E34:E50 E12:E29">
+  <conditionalFormatting sqref="E53:E59 E2:E10 E34:E50 E12:E29">
     <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
       <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D59:D61">
+  <conditionalFormatting sqref="D60:D62">
     <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
@@ -4214,7 +4266,7 @@
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E59:E61">
+  <conditionalFormatting sqref="E60:E62">
     <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"DNP"</formula>
     </cfRule>

</xml_diff>

<commit_message>
rev_f: more BOM fixes
 - Remove duplicate C20 entry
 - Add B1 as DNP entry
 - C71 and C72, while both 10uF, are 0402 and 0603 packages :/
</commit_message>
<xml_diff>
--- a/hardware/tottag/rev_f/tottag_bom.xlsx
+++ b/hardware/tottag/rev_f/tottag_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/code/lab11/totternary/hardware/tottag/rev_f/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D57CB6C-B24E-E441-9E9B-ADB8E735D85A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E418EE5F-CAF5-C143-B5FD-2A0E514D772F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="18760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tottag_bom" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="394">
   <si>
     <t>Qty</t>
   </si>
@@ -255,9 +255,6 @@
     <t>C0402C101J5RACAUTO</t>
   </si>
   <si>
-    <t>C19,C20</t>
-  </si>
-  <si>
     <t>330pF</t>
   </si>
   <si>
@@ -1086,9 +1083,6 @@
     <t>C60,C61,C62,C63,C64,C65,C66,C67,C68,C69,C70</t>
   </si>
   <si>
-    <t>C71,C72</t>
-  </si>
-  <si>
     <t>C73</t>
   </si>
   <si>
@@ -1180,6 +1174,39 @@
   </si>
   <si>
     <t>535-9543-1-ND</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>MS518SE</t>
+  </si>
+  <si>
+    <t>A small, low leakage rechargeable battery for RTC backup</t>
+  </si>
+  <si>
+    <t>FL35E</t>
+  </si>
+  <si>
+    <t>Coin, 5.8mm 3V Lithium Battery Rechargeable (Secondary) 3.4mAh</t>
+  </si>
+  <si>
+    <t>728-1054-ND</t>
+  </si>
+  <si>
+    <t>Seiko Instruments</t>
+  </si>
+  <si>
+    <t>MS518SE-FL35E</t>
+  </si>
+  <si>
+    <t>C72</t>
+  </si>
+  <si>
+    <t>C71</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1314,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1981,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L58" sqref="L58"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2390,7 +2432,7 @@
         <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>30</v>
@@ -2405,19 +2447,19 @@
         <v>33</v>
       </c>
       <c r="I11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K11" t="s">
         <v>42</v>
       </c>
       <c r="L11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="M11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="N11"/>
     </row>
@@ -2426,7 +2468,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>383</v>
       </c>
       <c r="C12" t="s">
         <v>72</v>
@@ -2463,10 +2505,10 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>30</v>
@@ -2482,16 +2524,16 @@
         <v>33</v>
       </c>
       <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="K13" t="s">
         <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N13"/>
     </row>
@@ -2500,10 +2542,10 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>16</v>
@@ -2519,16 +2561,16 @@
         <v>33</v>
       </c>
       <c r="I14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="K14" t="s">
         <v>64</v>
       </c>
       <c r="L14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N14"/>
     </row>
@@ -2537,10 +2579,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>30</v>
@@ -2556,16 +2598,16 @@
         <v>33</v>
       </c>
       <c r="I15" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="K15" t="s">
         <v>64</v>
       </c>
       <c r="L15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N15"/>
     </row>
@@ -2574,10 +2616,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>30</v>
@@ -2593,16 +2635,16 @@
         <v>33</v>
       </c>
       <c r="I16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="K16" t="s">
         <v>91</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>92</v>
-      </c>
-      <c r="L16" t="s">
-        <v>93</v>
       </c>
       <c r="N16"/>
     </row>
@@ -2611,10 +2653,10 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>30</v>
@@ -2630,16 +2672,16 @@
         <v>33</v>
       </c>
       <c r="I17" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="K17" t="s">
         <v>96</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>97</v>
-      </c>
-      <c r="L17" t="s">
-        <v>98</v>
       </c>
       <c r="N17"/>
     </row>
@@ -2648,10 +2690,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>30</v>
@@ -2667,16 +2709,16 @@
         <v>33</v>
       </c>
       <c r="I18" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="K18" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18" t="s">
         <v>101</v>
-      </c>
-      <c r="K18" t="s">
-        <v>97</v>
-      </c>
-      <c r="L18" t="s">
-        <v>102</v>
       </c>
       <c r="N18"/>
     </row>
@@ -2685,10 +2727,10 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>30</v>
@@ -2704,208 +2746,196 @@
         <v>33</v>
       </c>
       <c r="I19" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="K19" t="s">
         <v>42</v>
       </c>
       <c r="L19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>353</v>
+        <v>393</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="H20" t="s">
         <v>33</v>
       </c>
-      <c r="I20" t="s">
-        <v>110</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="K20" t="s">
-        <v>42</v>
-      </c>
-      <c r="L20" t="s">
-        <v>112</v>
-      </c>
+      <c r="J20" s="8"/>
       <c r="N20" s="10" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="14" x14ac:dyDescent="0.15">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>354</v>
+        <v>392</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" t="s">
         <v>108</v>
-      </c>
-      <c r="G21" t="s">
-        <v>109</v>
       </c>
       <c r="H21" t="s">
         <v>33</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K21" t="s">
         <v>42</v>
       </c>
       <c r="L21" t="s">
-        <v>116</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N21"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="14" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>352</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G22" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="H22" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="K22" t="s">
-        <v>125</v>
+        <v>42</v>
       </c>
       <c r="L22" t="s">
-        <v>126</v>
+        <v>115</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="N22"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G23" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H23" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I23" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="K23" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="L23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N23"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G24" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H24" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I24" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="K24" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="L24" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="N24"/>
     </row>
@@ -2914,35 +2944,35 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="G25" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H25" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I25" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="K25" t="s">
+        <v>139</v>
+      </c>
+      <c r="L25" t="s">
         <v>140</v>
-      </c>
-      <c r="L25" t="s">
-        <v>147</v>
       </c>
       <c r="N25"/>
     </row>
@@ -2951,35 +2981,35 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G26" t="s">
-        <v>32</v>
+        <v>140</v>
       </c>
       <c r="H26" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="I26" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="K26" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="L26" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="N26"/>
     </row>
@@ -2988,35 +3018,35 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C27" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G27" t="s">
         <v>32</v>
       </c>
       <c r="H27" t="s">
+        <v>150</v>
+      </c>
+      <c r="I27" t="s">
         <v>151</v>
       </c>
-      <c r="I27" t="s">
-        <v>158</v>
-      </c>
       <c r="J27" s="8" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="K27" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="L27" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="N27"/>
     </row>
@@ -3025,219 +3055,220 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C28" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="G28" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="H28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I28" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="K28" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="L28" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="N28"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0</v>
+        <v>160</v>
+      </c>
+      <c r="C29" t="s">
+        <v>161</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G29" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="H29" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="I29" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="K29" t="s">
-        <v>173</v>
+        <v>91</v>
       </c>
       <c r="L29" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="N29"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C30" s="7">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" t="s">
         <v>168</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>169</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>170</v>
       </c>
-      <c r="I30" t="s">
-        <v>176</v>
-      </c>
       <c r="J30" s="8" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="K30" t="s">
-        <v>97</v>
+        <v>172</v>
       </c>
       <c r="L30" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="N30"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C31" s="7">
-        <v>470</v>
+        <v>270</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" t="s">
         <v>168</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>169</v>
       </c>
-      <c r="H31" t="s">
-        <v>170</v>
-      </c>
       <c r="I31" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="J31" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="K31" t="s">
-        <v>182</v>
+        <v>96</v>
       </c>
       <c r="L31" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="N31"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
-      </c>
-      <c r="C32" t="s">
-        <v>185</v>
+        <v>178</v>
+      </c>
+      <c r="C32" s="7">
+        <v>470</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" t="s">
         <v>168</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>169</v>
       </c>
-      <c r="H32" t="s">
-        <v>170</v>
-      </c>
       <c r="I32" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="K32" t="s">
+        <v>181</v>
+      </c>
+      <c r="L32" t="s">
         <v>182</v>
-      </c>
-      <c r="L32" t="s">
-        <v>188</v>
       </c>
       <c r="N32"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C33" t="s">
-        <v>356</v>
+        <v>184</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E33" s="5"/>
       <c r="F33" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" t="s">
         <v>168</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>169</v>
       </c>
-      <c r="H33" t="s">
-        <v>170</v>
-      </c>
       <c r="I33" t="s">
-        <v>359</v>
-      </c>
-      <c r="J33" t="s">
-        <v>357</v>
+        <v>185</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="K33" t="s">
-        <v>27</v>
+        <v>181</v>
       </c>
       <c r="L33" t="s">
-        <v>358</v>
+        <v>187</v>
       </c>
       <c r="N33"/>
     </row>
@@ -3246,220 +3277,219 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>360</v>
+        <v>188</v>
       </c>
       <c r="C34" t="s">
-        <v>190</v>
+        <v>354</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E34" s="5"/>
+        <v>16</v>
+      </c>
       <c r="F34" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" t="s">
         <v>168</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>169</v>
       </c>
-      <c r="H34" t="s">
-        <v>170</v>
-      </c>
       <c r="I34" t="s">
-        <v>191</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>192</v>
+        <v>357</v>
+      </c>
+      <c r="J34" t="s">
+        <v>355</v>
       </c>
       <c r="K34" t="s">
-        <v>173</v>
+        <v>27</v>
       </c>
       <c r="L34" t="s">
-        <v>193</v>
+        <v>356</v>
       </c>
       <c r="N34"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C35" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" t="s">
         <v>168</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>169</v>
       </c>
-      <c r="H35" t="s">
-        <v>170</v>
-      </c>
       <c r="I35" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L35" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="N35"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C36" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" t="s">
         <v>168</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>169</v>
       </c>
-      <c r="H36" t="s">
-        <v>170</v>
-      </c>
       <c r="I36" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="K36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L36" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="N36"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>360</v>
       </c>
       <c r="C37" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" t="s">
         <v>168</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>169</v>
       </c>
-      <c r="H37" t="s">
-        <v>170</v>
-      </c>
       <c r="I37" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="K37" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="L37" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="N37"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>363</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" t="s">
         <v>168</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>169</v>
       </c>
-      <c r="H38" t="s">
-        <v>170</v>
-      </c>
       <c r="I38" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="K38" t="s">
-        <v>182</v>
+        <v>27</v>
       </c>
       <c r="L38" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="N38"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C39" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" t="s">
         <v>168</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>169</v>
       </c>
-      <c r="H39" t="s">
-        <v>170</v>
-      </c>
       <c r="I39" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="J39" s="8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="K39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L39" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="N39"/>
     </row>
@@ -3468,35 +3498,35 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" t="s">
         <v>168</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>169</v>
       </c>
-      <c r="H40" t="s">
-        <v>170</v>
-      </c>
       <c r="I40" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J40" s="8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="K40" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="L40" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="N40"/>
     </row>
@@ -3505,35 +3535,35 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>219</v>
+        <v>363</v>
       </c>
       <c r="C41" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" t="s">
-        <v>220</v>
+        <v>167</v>
       </c>
       <c r="G41" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
       <c r="H41" t="s">
-        <v>222</v>
+        <v>169</v>
       </c>
       <c r="I41" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="K41" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
       <c r="L41" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="N41"/>
     </row>
@@ -3542,35 +3572,35 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C42" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G42" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="H42" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="I42" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="K42" t="s">
-        <v>231</v>
+        <v>91</v>
       </c>
       <c r="L42" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="N42"/>
     </row>
@@ -3579,35 +3609,35 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="C43" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="G43" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="H43" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="I43" t="s">
-        <v>237</v>
-      </c>
-      <c r="J43" t="s">
-        <v>238</v>
+        <v>228</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>229</v>
       </c>
       <c r="K43" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="L43" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="N43"/>
     </row>
@@ -3616,35 +3646,35 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C44" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G44" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H44" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="I44" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="J44" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="K44" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="L44" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="N44"/>
     </row>
@@ -3653,35 +3683,35 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C45" t="s">
-        <v>366</v>
+        <v>240</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" t="s">
-        <v>366</v>
+        <v>240</v>
       </c>
       <c r="G45" t="s">
-        <v>367</v>
+        <v>241</v>
       </c>
       <c r="H45" t="s">
-        <v>368</v>
+        <v>242</v>
       </c>
       <c r="I45" t="s">
-        <v>372</v>
+        <v>243</v>
       </c>
       <c r="J45" t="s">
-        <v>369</v>
+        <v>244</v>
       </c>
       <c r="K45" t="s">
-        <v>371</v>
+        <v>245</v>
       </c>
       <c r="L45" t="s">
-        <v>370</v>
+        <v>246</v>
       </c>
       <c r="N45"/>
     </row>
@@ -3690,35 +3720,35 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C46" t="s">
-        <v>250</v>
+        <v>364</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" t="s">
-        <v>250</v>
+        <v>364</v>
       </c>
       <c r="G46" t="s">
-        <v>251</v>
+        <v>365</v>
       </c>
       <c r="H46" t="s">
-        <v>252</v>
+        <v>366</v>
       </c>
       <c r="I46" t="s">
-        <v>253</v>
+        <v>370</v>
       </c>
       <c r="J46" t="s">
-        <v>254</v>
+        <v>367</v>
       </c>
       <c r="K46" t="s">
-        <v>255</v>
+        <v>369</v>
       </c>
       <c r="L46" t="s">
-        <v>250</v>
+        <v>368</v>
       </c>
       <c r="N46"/>
     </row>
@@ -3727,35 +3757,35 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C47" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="G47" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H47" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="I47" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="J47" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="K47" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="L47" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="N47"/>
     </row>
@@ -3764,35 +3794,35 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C48" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="G48" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="H48" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="I48" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="J48" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="K48" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="L48" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="N48"/>
     </row>
@@ -3801,35 +3831,35 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="C49" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="G49" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="H49" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I49" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="J49" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="K49" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="L49" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="N49"/>
     </row>
@@ -3838,35 +3868,35 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C50" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="G50" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="H50" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="I50" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="J50" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="K50" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="L50" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="N50"/>
     </row>
@@ -3875,35 +3905,35 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C51" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="G51" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="H51" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="I51" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="J51" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="K51" t="s">
-        <v>246</v>
+        <v>284</v>
       </c>
       <c r="L51" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="N51"/>
     </row>
@@ -3912,34 +3942,35 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>373</v>
+        <v>286</v>
       </c>
       <c r="C52" t="s">
-        <v>374</v>
+        <v>287</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="E52" s="5"/>
       <c r="F52" t="s">
-        <v>374</v>
+        <v>287</v>
       </c>
       <c r="G52" t="s">
-        <v>375</v>
+        <v>288</v>
       </c>
       <c r="H52" t="s">
-        <v>376</v>
+        <v>289</v>
       </c>
       <c r="I52" t="s">
-        <v>379</v>
+        <v>290</v>
       </c>
       <c r="J52" t="s">
-        <v>377</v>
+        <v>291</v>
       </c>
       <c r="K52" t="s">
-        <v>378</v>
+        <v>245</v>
       </c>
       <c r="L52" t="s">
-        <v>374</v>
+        <v>292</v>
       </c>
       <c r="N52"/>
     </row>
@@ -3948,35 +3979,34 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>294</v>
+        <v>371</v>
       </c>
       <c r="C53" t="s">
-        <v>295</v>
+        <v>372</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E53" s="5"/>
       <c r="F53" t="s">
-        <v>296</v>
+        <v>372</v>
       </c>
       <c r="G53" t="s">
-        <v>297</v>
+        <v>373</v>
       </c>
       <c r="H53" t="s">
-        <v>298</v>
+        <v>374</v>
       </c>
       <c r="I53" t="s">
-        <v>299</v>
+        <v>377</v>
       </c>
       <c r="J53" t="s">
-        <v>300</v>
+        <v>375</v>
       </c>
       <c r="K53" t="s">
-        <v>154</v>
+        <v>376</v>
       </c>
       <c r="L53" t="s">
-        <v>296</v>
+        <v>372</v>
       </c>
       <c r="N53"/>
     </row>
@@ -3985,35 +4015,35 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C54" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="G54" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="H54" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="I54" t="s">
-        <v>305</v>
-      </c>
-      <c r="J54" s="8" t="s">
-        <v>306</v>
+        <v>298</v>
+      </c>
+      <c r="J54" t="s">
+        <v>299</v>
       </c>
       <c r="K54" t="s">
-        <v>307</v>
+        <v>153</v>
       </c>
       <c r="L54" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="N54"/>
     </row>
@@ -4022,35 +4052,35 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C55" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="G55" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="H55" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="I55" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="J55" s="8" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="K55" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="L55" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="N55"/>
     </row>
@@ -4059,35 +4089,35 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C56" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="G56" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="H56" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="I56" t="s">
-        <v>320</v>
-      </c>
-      <c r="J56" t="s">
-        <v>321</v>
+        <v>313</v>
+      </c>
+      <c r="J56" s="8" t="s">
+        <v>314</v>
       </c>
       <c r="K56" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="L56" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="N56"/>
     </row>
@@ -4096,242 +4126,319 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>380</v>
+        <v>317</v>
       </c>
       <c r="C57" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" t="s">
-        <v>382</v>
+        <v>302</v>
       </c>
       <c r="G57" t="s">
-        <v>381</v>
+        <v>302</v>
       </c>
       <c r="H57" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="I57" t="s">
-        <v>383</v>
+        <v>319</v>
       </c>
       <c r="J57" t="s">
-        <v>384</v>
+        <v>320</v>
       </c>
       <c r="K57" t="s">
-        <v>154</v>
+        <v>306</v>
       </c>
       <c r="L57" t="s">
-        <v>382</v>
+        <v>321</v>
       </c>
       <c r="N57"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A58">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>323</v>
+        <v>378</v>
       </c>
       <c r="C58" t="s">
-        <v>324</v>
-      </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="5" t="s">
-        <v>325</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="5"/>
       <c r="F58" t="s">
-        <v>324</v>
+        <v>380</v>
       </c>
       <c r="G58" t="s">
-        <v>326</v>
+        <v>379</v>
       </c>
       <c r="H58" t="s">
-        <v>327</v>
+        <v>297</v>
+      </c>
+      <c r="I58" t="s">
+        <v>381</v>
+      </c>
+      <c r="J58" t="s">
+        <v>382</v>
+      </c>
+      <c r="K58" t="s">
+        <v>153</v>
+      </c>
+      <c r="L58" t="s">
+        <v>380</v>
       </c>
       <c r="N58"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A59">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C59" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="F59" t="s">
+        <v>323</v>
+      </c>
+      <c r="G59" t="s">
         <v>325</v>
       </c>
-      <c r="F59" t="s">
-        <v>329</v>
-      </c>
-      <c r="G59" t="s">
-        <v>330</v>
+      <c r="H59" t="s">
+        <v>326</v>
       </c>
       <c r="N59"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A60">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C60" t="s">
-        <v>332</v>
-      </c>
-      <c r="D60" s="5"/>
-      <c r="E60" s="4" t="s">
-        <v>325</v>
+        <v>328</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5" t="s">
+        <v>324</v>
       </c>
       <c r="F60" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G60" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="N60"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C61" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F61" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G61" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="N61"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C62" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F62" t="s">
+        <v>334</v>
+      </c>
+      <c r="G62" t="s">
+        <v>335</v>
+      </c>
+      <c r="N62"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>336</v>
+      </c>
+      <c r="C63" t="s">
+        <v>337</v>
+      </c>
+      <c r="D63" s="5"/>
+      <c r="E63" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F63" t="s">
+        <v>337</v>
+      </c>
+      <c r="G63" t="s">
         <v>338</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H63" t="s">
         <v>339</v>
       </c>
-      <c r="H62" t="s">
-        <v>340</v>
-      </c>
-      <c r="N62"/>
+      <c r="N63"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
+        <v>384</v>
+      </c>
+      <c r="C64" t="s">
+        <v>385</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="F64" t="s">
+        <v>385</v>
+      </c>
+      <c r="G64" t="s">
+        <v>387</v>
+      </c>
+      <c r="H64" t="s">
+        <v>386</v>
+      </c>
+      <c r="I64" t="s">
+        <v>388</v>
+      </c>
+      <c r="J64" t="s">
+        <v>389</v>
+      </c>
+      <c r="K64" t="s">
+        <v>390</v>
+      </c>
+      <c r="L64" t="s">
+        <v>391</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10 D34:D50 D12:D29 D53:D59">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+  <conditionalFormatting sqref="D2:D10 D35:D51 D54:D60 D12:D30">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53:E59 E2:E10 E34:E50 E12:E29">
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+  <conditionalFormatting sqref="E54:E60 E2:E10 E35:E51 E12:E30">
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
       <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D62">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
+  <conditionalFormatting sqref="D61:D63">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E60:E62">
-    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
+  <conditionalFormatting sqref="E61:E63">
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
       <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30:D31">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+  <conditionalFormatting sqref="D31:D32">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30:E31">
-    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
+  <conditionalFormatting sqref="E31:E32">
+    <cfRule type="cellIs" dxfId="13" priority="17" operator="equal">
       <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+  <conditionalFormatting sqref="D33">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="19" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
+  <conditionalFormatting sqref="E33">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
+  <conditionalFormatting sqref="D52">
+    <cfRule type="cellIs" dxfId="9" priority="21" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="22" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="cellIs" dxfId="6" priority="22" operator="equal">
+  <conditionalFormatting sqref="E52">
+    <cfRule type="cellIs" dxfId="7" priority="23" operator="equal">
       <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="D34">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="D53">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"DNP"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>